<commit_message>
Update Emotional-Vocab-Pos.xlsx: 자부실 -> 자부심
</commit_message>
<xml_diff>
--- a/data/Emotional-Vocab-Pos.xlsx
+++ b/data/Emotional-Vocab-Pos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/PycharmProjects/WiseNLU-user/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65863157-9313-5047-88A1-120E7FB69788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7483DB5E-BAFC-4143-9102-9EE10D93E4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5540" yWindow="3520" windowWidth="27700" windowHeight="16880" xr2:uid="{4FB77EC3-1A6B-154F-8E90-DC2475B6D259}"/>
   </bookViews>
@@ -186,10 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자부실</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>자긍심</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -775,6 +771,10 @@
   </si>
   <si>
     <t>순번</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자부심</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1161,18 +1161,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C874ED-51BF-4144-BC5A-5C735F4F1E7A}">
   <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1188,7 +1188,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1196,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1220,7 +1220,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1228,7 +1228,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1236,7 +1236,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1244,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1252,7 +1252,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1260,7 +1260,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1268,7 +1268,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1276,7 +1276,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1284,7 +1284,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1292,7 +1292,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1300,7 +1300,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1308,7 +1308,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1316,7 +1316,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1324,7 +1324,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1332,7 +1332,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1340,7 +1340,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1348,7 +1348,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1356,7 +1356,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1364,7 +1364,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1372,7 +1372,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1380,7 +1380,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1388,7 +1388,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1396,7 +1396,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1404,7 +1404,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1412,7 +1412,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1420,7 +1420,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1428,7 +1428,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1436,7 +1436,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1444,7 +1444,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1452,7 +1452,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1460,7 +1460,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1468,7 +1468,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1476,7 +1476,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1484,7 +1484,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1492,7 +1492,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1500,7 +1500,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1508,7 +1508,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1516,7 +1516,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1524,7 +1524,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1532,7 +1532,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1540,7 +1540,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1548,7 +1548,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1556,7 +1556,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1564,7 +1564,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1572,7 +1572,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1580,7 +1580,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1588,7 +1588,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1596,7 +1596,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1604,7 +1604,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1612,7 +1612,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1620,7 +1620,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1628,7 +1628,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1636,7 +1636,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1644,7 +1644,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1652,7 +1652,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1660,7 +1660,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1668,7 +1668,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1676,7 +1676,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1684,7 +1684,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1692,7 +1692,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1700,7 +1700,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1708,7 +1708,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1716,7 +1716,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1724,7 +1724,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1732,7 +1732,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1740,7 +1740,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1748,7 +1748,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1756,7 +1756,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1764,7 +1764,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1772,7 +1772,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1780,7 +1780,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1788,7 +1788,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1796,7 +1796,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1804,7 +1804,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1812,7 +1812,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1820,7 +1820,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1828,7 +1828,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1836,7 +1836,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1844,7 +1844,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1852,7 +1852,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1860,7 +1860,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1868,7 +1868,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1876,7 +1876,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1884,7 +1884,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1892,7 +1892,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1900,7 +1900,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1908,7 +1908,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1916,7 +1916,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1924,7 +1924,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1932,7 +1932,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1940,7 +1940,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1948,7 +1948,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1956,7 +1956,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1964,7 +1964,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1972,7 +1972,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1980,7 +1980,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1988,7 +1988,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1996,7 +1996,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2004,7 +2004,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2012,7 +2012,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2020,7 +2020,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2028,7 +2028,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2036,7 +2036,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2044,7 +2044,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2052,7 +2052,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2060,7 +2060,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2068,7 +2068,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2076,7 +2076,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2084,7 +2084,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2092,7 +2092,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2100,7 +2100,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2108,7 +2108,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2116,7 +2116,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2124,7 +2124,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2132,7 +2132,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2140,7 +2140,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2148,7 +2148,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2156,7 +2156,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2164,7 +2164,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2172,7 +2172,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2180,7 +2180,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2188,7 +2188,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2196,7 +2196,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2204,7 +2204,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2212,7 +2212,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2220,7 +2220,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2228,7 +2228,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2236,7 +2236,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2244,7 +2244,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2252,7 +2252,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2260,7 +2260,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2268,7 +2268,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2276,7 +2276,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2284,7 +2284,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2292,7 +2292,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2300,7 +2300,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2308,7 +2308,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2316,7 +2316,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2324,7 +2324,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2332,7 +2332,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2340,7 +2340,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2348,7 +2348,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2356,7 +2356,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2364,7 +2364,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2372,7 +2372,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>37</v>
+        <v>184</v>
       </c>
     </row>
     <row r="152" spans="1:2">

</xml_diff>